<commit_message>
added first conception protocoll, updated todo
</commit_message>
<xml_diff>
--- a/ToDo_list.xlsx
+++ b/ToDo_list.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>Prio</t>
   </si>
@@ -114,18 +114,12 @@
     <t>Level in Unity zusammensetzen</t>
   </si>
   <si>
-    <t>Avatar testen und ggf. anpassen</t>
-  </si>
-  <si>
     <t>Konzept überarbeiten, Spielziel, Story, wie bringe ich den Spieler zum lernen etc.</t>
   </si>
   <si>
     <t>Balancing</t>
   </si>
   <si>
-    <t>Gestentool trainieren und Paramterwerte anpassen</t>
-  </si>
-  <si>
     <t>Installation Testaufbau</t>
   </si>
   <si>
@@ -135,35 +129,41 @@
     <t>Showreel vorbereiten</t>
   </si>
   <si>
-    <t>Erste primitive Level Assets bauen</t>
-  </si>
-  <si>
     <t>Rene, Robert</t>
   </si>
   <si>
     <t>Rene</t>
   </si>
   <si>
-    <t>Implementierung d. Gestentools nach erstem Test in Unity anpassen</t>
-  </si>
-  <si>
-    <t>Gestentool um Features erweitern</t>
-  </si>
-  <si>
-    <t>KinecticSpace in Unity implementieren</t>
-  </si>
-  <si>
     <t>Konzepte erarbeiten die mit normalen Spielerlebnis nichts zu tun haben (z.B .Blur d. Kamera)</t>
   </si>
   <si>
-    <t>Avatar soll links / rechts hüpfen</t>
+    <t>Erste Level Assets bauen</t>
+  </si>
+  <si>
+    <t>Avatar mit Funktionalität erfüllen mit Castle testen und ggf. anpassen</t>
+  </si>
+  <si>
+    <t>Testlevel in Unity bauen</t>
+  </si>
+  <si>
+    <t>KinecticSpace ggf. anpassen</t>
+  </si>
+  <si>
+    <t>Gesten trainieren</t>
+  </si>
+  <si>
+    <t>Woche vom 10.</t>
+  </si>
+  <si>
+    <t>KinecticSpace in Unity zum Laufen bekommen / Hardcode x,y herausfinden / Doku</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -186,8 +186,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -206,6 +219,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -219,13 +244,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -508,15 +538,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:E30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="78.109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -709,7 +739,7 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C16" t="s">
         <v>23</v>
@@ -717,14 +747,14 @@
       <c r="D16" s="3">
         <v>42493</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="10"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>16</v>
@@ -732,29 +762,34 @@
       <c r="D17" s="3">
         <v>42488</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="9"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>3</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D18" s="3"/>
-      <c r="E18" s="2"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B19" t="s">
         <v>29</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
-      </c>
-      <c r="D19" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="D19" s="7">
+        <v>42493</v>
+      </c>
       <c r="E19" s="2"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
@@ -762,12 +797,14 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D20" s="3">
+        <v>42500</v>
+      </c>
       <c r="E20" s="2"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
@@ -780,30 +817,39 @@
       <c r="C21" t="s">
         <v>12</v>
       </c>
-      <c r="D21" s="3"/>
+      <c r="D21" s="3">
+        <v>42507</v>
+      </c>
       <c r="E21" s="2"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="C22" t="s">
+        <v>12</v>
+      </c>
+      <c r="D22" s="3">
+        <v>42493</v>
+      </c>
       <c r="E22" s="2"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B23" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>25</v>
       </c>
-      <c r="D23" s="3"/>
+      <c r="D23" s="3">
+        <v>42500</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
@@ -811,9 +857,14 @@
         <v>1</v>
       </c>
       <c r="B24" t="s">
-        <v>34</v>
-      </c>
-      <c r="D24" s="3"/>
+        <v>33</v>
+      </c>
+      <c r="C24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>44</v>
+      </c>
       <c r="E24" s="2"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
@@ -821,63 +872,59 @@
         <v>2</v>
       </c>
       <c r="B25" t="s">
-        <v>42</v>
+        <v>43</v>
+      </c>
+      <c r="C25" t="s">
+        <v>16</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="2"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B26" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="2"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B27" t="s">
+        <v>34</v>
+      </c>
+      <c r="C27" t="s">
+        <v>9</v>
+      </c>
+      <c r="D27" s="3">
+        <v>42493</v>
+      </c>
+      <c r="E27" s="2"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C27" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="3"/>
-      <c r="E27" s="2"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <v>3</v>
-      </c>
-      <c r="B28" t="s">
-        <v>36</v>
-      </c>
-      <c r="D28" s="3"/>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" s="3">
+        <v>42549</v>
+      </c>
       <c r="E28" s="2"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <v>3</v>
-      </c>
       <c r="B29" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="D29" s="3"/>
-      <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <v>3</v>
-      </c>
-      <c r="B30" t="s">
-        <v>33</v>
-      </c>
       <c r="D30" s="3"/>
-      <c r="E30" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>